<commit_message>
Remove duplicated chart in the Excel file
</commit_message>
<xml_diff>
--- a/Interview/analysis/visualization.xlsx
+++ b/Interview/analysis/visualization.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Academic\Northeastern\GSND 5130\GP3\Interview\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F7258A-CCE4-4B13-AF32-EA7D055CC6CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12DEFB4-ABB6-4CE6-9936-9B3736C7A3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accent" sheetId="1" r:id="rId1"/>
@@ -274,11 +274,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -287,7 +286,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2526,552 +2525,6 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:sysClr val="windowText" lastClr="000000">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:sysClr>
-                </a:solidFill>
-              </a:rPr>
-              <a:t>Realization of &lt;o&gt;</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>vowel!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Asia</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>vowel!$K$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>o_o</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>o_ɔ</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>o_əʊ</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>vowel!$K$2:$M$2</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.75</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-571D-433E-A762-E98D8AAB7439}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>vowel!$A$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Middle East</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>vowel!$K$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>o_o</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>o_ɔ</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>o_əʊ</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>vowel!$K$3:$M$3</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.42857142857142799</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.28571428571428498</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.28571428571428498</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-571D-433E-A762-E98D8AAB7439}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>vowel!$A$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Southern Europe</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>vowel!$K$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>o_o</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>o_ɔ</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>o_əʊ</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>vowel!$K$4:$M$4</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.6</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-571D-433E-A762-E98D8AAB7439}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>vowel!$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Central and Eastern Europe</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>vowel!$K$1:$M$1</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>o_o</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>o_ɔ</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>o_əʊ</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>vowel!$K$5:$M$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16666666666666599</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.33333333333333298</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-571D-433E-A762-E98D8AAB7439}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1145915535"/>
-        <c:axId val="1145916015"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1145915535"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1145916015"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1145916015"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1145915535"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
               <a:rPr lang="en-US"/>
               <a:t>Realization of &lt;o&gt;</a:t>
             </a:r>
@@ -3578,7 +3031,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4358,46 +3811,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6914,509 +6327,6 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7965,15 +6875,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>60325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8077,50 +6987,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>282575</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>158750</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05CA94C5-4A73-9BA7-CD06-1A9592F6CE54}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>263525</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>234950</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
@@ -8141,7 +7015,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8149,14 +7023,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>111125</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>126999</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
@@ -8177,7 +7051,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -8463,57 +7337,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>0.27272727272727199</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>8.3333332999999996E-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>0.29032258064516098</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.12962962962962901</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0.42857142857142799</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>0.30555555555555503</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>0.36363636363636298</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.29166666666666602</v>
       </c>
     </row>
@@ -8527,8 +7401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0009C037-047F-445D-9964-93F61EFCF014}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8538,117 +7412,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>0.66666666666666596</v>
       </c>
-      <c r="C2" s="12">
+      <c r="C2" s="11">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>0.5</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.5</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>0.66666666666666596</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="11">
         <v>0.33333333333333298</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>0.83333333333333304</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>0.16666666666666599</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>0.6</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0.4</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.6</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -8662,8 +7536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{266C3ED6-BFCE-4CBD-BC06-F1B73A23708F}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y18" sqref="Y18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8673,252 +7547,252 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="I1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="13">
         <v>0.5625</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>0.1875</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>6.25E-2</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="3">
         <v>0.125</v>
       </c>
-      <c r="I2" s="14">
+      <c r="I2" s="13">
         <v>0</v>
       </c>
-      <c r="J2" s="4">
+      <c r="J2" s="3">
         <v>1</v>
       </c>
-      <c r="K2" s="14">
+      <c r="K2" s="13">
         <v>0.25</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2" s="2">
         <v>0</v>
       </c>
-      <c r="M2" s="4">
+      <c r="M2" s="3">
         <v>0.75</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" s="2">
         <v>0.66666666666666596</v>
       </c>
-      <c r="O2" s="3">
+      <c r="O2" s="2">
         <v>0.22222222222222199</v>
       </c>
-      <c r="P2" s="4">
+      <c r="P2" s="3">
         <v>0.11111111111111099</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="13">
         <v>0.33333333333333298</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>0.11111111111111099</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>0.22222222222222199</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>0.22222222222222199</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <v>5.5555555555555497E-2</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>5.5555555555555497E-2</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>0.6</v>
       </c>
-      <c r="J3" s="4">
+      <c r="J3" s="3">
         <v>0.4</v>
       </c>
-      <c r="K3" s="14">
+      <c r="K3" s="13">
         <v>0.42857142857142799</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="2">
         <v>0.28571428571428498</v>
       </c>
-      <c r="M3" s="4">
+      <c r="M3" s="3">
         <v>0.28571428571428498</v>
       </c>
-      <c r="N3" s="3">
+      <c r="N3" s="2">
         <v>0.66666666666666596</v>
       </c>
-      <c r="O3" s="3">
+      <c r="O3" s="2">
         <v>0.22222222222222199</v>
       </c>
-      <c r="P3" s="4">
+      <c r="P3" s="3">
         <v>0.11111111111111099</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>0.5</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="2">
         <v>0</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <v>0</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>0.16666666666666599</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <v>0.25</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>0</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="3">
         <v>8.3333333333333301E-2</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="13">
         <v>0.66666666666666596</v>
       </c>
-      <c r="J4" s="4">
+      <c r="J4" s="3">
         <v>0.33333333333333298</v>
       </c>
-      <c r="K4" s="14">
+      <c r="K4" s="13">
         <v>0.2</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="2">
         <v>0.2</v>
       </c>
-      <c r="M4" s="4">
+      <c r="M4" s="3">
         <v>0.6</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N4" s="2">
         <v>0.33333333333333298</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O4" s="2">
         <v>0.33333333333333298</v>
       </c>
-      <c r="P4" s="4">
+      <c r="P4" s="3">
         <v>0.33333333333333298</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>0.4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.2</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.3</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.1</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>0</v>
       </c>
-      <c r="I5" s="15">
+      <c r="I5" s="14">
         <v>0.5</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>0.5</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="14">
         <v>0.5</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>0.16666666666666599</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>0.33333333333333298</v>
       </c>
-      <c r="N5" s="5">
+      <c r="N5" s="4">
         <v>0</v>
       </c>
-      <c r="O5" s="5">
+      <c r="O5" s="4">
         <v>0</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>